<commit_message>
update data day 05/10/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/ketqua2.xlsx
+++ b/Data/Draft/ketqua2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,37 +436,47 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>author_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>content</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>author_id</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>label</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>link</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>comment_list</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>link</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vietnamnet.vn</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>HÀ NỘI: XƯỞNG TÁI CHẾ NHỰA BỐC CHÁY DỮ DỘI, 1 NGƯỜI KHÔNG QUA KHỎI 
 Chiều 28/9, Công an TP Hà Nội thông tin về vụ cháy xưởng tái chế nhựa khiến 1 người không qua khỏi, xảy ra tại đội 12, khu chùa Rừng - Miền Bãi, xã Dương Liễu, huyện Hoài Đức.
@@ -479,44 +489,504 @@
 #Vietnamnet #Thờisự #PT</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>https://www.facebook.com/vietnamnet.vn</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>[
-    {
-        "comment_id": "c4",
-        "author": "Vietnamnet.vn",
-        "content": "Xem bài viết này trên Vietnamnet:"
-    },
-    {
-        "comment_id": "c5",
-        "author": "Tú Hoàng",
-        "content": "A di đà Phật"
-    },
-    {
-        "comment_id": "c6",
-        "author": "Hồ Mỹ Liên",
-        "content": "Nam mô a di đà phật"
-    }
-]</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/vietnamnet.vn/posts/553740453703786?ref=embed_post</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PHẦN CÒN LẠI CỦA CẦU PHONG CHÂU CŨNG CÓ NGUY CƠ BỊ ĐỔ SẬP 
+Theo Công an tỉnh Phú Thọ, trong quá trình điều tra nguyên nhân vụ đổ trụ cầu T7 và 2 nhịp N6 và N7 của cầu Phong Châu, đơn vị nhận thấy mặt cầu nhịp số 5 (phần cầu nối với huyện Lâm Thao) đã bị nghiêng ra ngoài phía lòng sông Hồng và có nguy cơ đổ sập cao.
+Ghi nhận của PV VietNamNet ngày 28/9, sau sự cố sập cầu Phong Châu, phía bờ huyện Lâm Thao còn lại trụ cầu T5, T6 và nhịp dàn thép 66m nối giữa 2 trụ trên. Phía bờ huyện Tam Nông còn lại trụ cầu T8. 
+Để đảm bảo an toàn tính mạng và tài sản của nhân dân quanh khu vực cầu Phong Châu, ngày 27/9, Sở GTVT tỉnh Phú Thọ đã có văn bản đề nghị Cục Đường bộ Việt Nam xem xét, cho ý kiến về phương án xử lý các nhịp cầu và các trụ cầu còn lại của cầu Phong Châu. 
+#Vietnamnet #Thờisự #PT</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vietnamnet.vn</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>TIN VUI: “ĐÀO, PHỞ VÀ PIANO” LÊN SÓNG VTV 
+"Đào Phở và Piano", bộ phim vừa được chọn đại diện cho điện ảnh Việt dự vòng sơ loại Oscar 2025 sẽ được phát sóng lúc 21h20 ngày 13/10/2024 trên VTV1 nhân dịp kỷ niệm 70 năm ngày Giải phóng Thủ đô.
+#Vietnamnet #Giảitrí #NL</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vietnamnet.vn</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>HƠN 100.000 CÂY Ở HÀ NỘI BỊ QUẬT ĐỔ DO BÃO YAGI 
+Sáng 28/9, tại hội nghị của Thường trực Chính phủ đánh giá, rút kinh nghiệm về công tác phòng, chống và khắc phục hậu quả bão Yagi, lãnh đạo TP Hà Nội cho biết, trong đợt bão lụt vừa qua, trên địa bàn có 4 người tuvong, 28 người bị thương.
+Hầu hết các địa phương trên địa bàn TP Hà Nội bị ảnh hưởng, thiệt hại về tài sản trong đợt bão lụt vừa qua. Thống kê cho thấy, bão lụt khiến trên 100 nghìn cây xanh bị gãy, đổ (bao gồm cây đô thị và các loại cây khác). Nông nghiệp là lĩnh vực bị ảnh hưởng lớn nhất với trên 23.000 ha lúa bị gãy, đổ, dập nát; 15.000 ha lúa bị ngập.
+Toàn TP Hà Nội cũng đã ghi nhận xảy ra khoảng 40 sự cố đê điều, trên 150 sự cố công trình thủy lợi cùng các sự cố, ảnh hưởng khác về ngập lụt…
+TP Hà Nội ước tính thiệt hại kinh tế (nhất là nông nghiệp) do cơn bão Yagi và mưa lũ sau bão là trên 2.287 tỷ đồng.
+ #Vietnamnet #Thờisự #NL</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vietnamnet.vn</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Bộ Y tế xử phạt Dược phẩm Nam Hà 70 triệu đồng vì sản xuất lô thuốc vi phạm chất lượng</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vietnamnet.vn</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>TÀU LẠI TRẬT BÁNH KHỎI ĐƯỜNG RAY KHI QUA THỪA THIÊN HUẾ, ĐÂY LÀ VỤ TRẬT BÁNH TÀU THỨ 5 TRONG 2 THÁNG QUA
+Đến 9h ngày 28/9, Công ty CP đường sắt Bình Trị Thiên (Tổng Công ty đường sắt Việt Nam) cho biết, đơn vị vừa khắc phục xong sự cố tàu chở hàng bị trật bánh khỏi đường ray khi đi qua địa phận thị trấn Lăng Cô (huyện Phú Lộc, tỉnh Thừa Thiên Huế).
+Trước đó, vào khoảng 3h10 sáng cùng ngày, đầu máy D19E-943 kéo 24 toa hàng container HH16T chạy trên đường sắt Bắc - Nam.
+Khi đoàn tàu đến khu gian Lăng Cô - Thừa Lưu, cách ga Lăng Cô gần 4km thì đầu máy của tàu bất ngờ bị trật bánh khỏi đường ray. Vị trí xảy ra sự cố nằm trên chính tuyến, khiến tuyến đường sắt tạm thời bị gián đoạn.
+Đáng nói, trong 2 tháng qua, ngành đường sắt ghi nhận nhiều vụ tàu bị trật bánh khỏi đường ray khi lưu thông qua địa phận huyện Phú Lộc. Mặc dù các vụ việc không gây thiệt hại về người nhưng ảnh hưởng đến quá trình vận hành, lưu thông của tuyến đường sắt Bắc – Nam.
+#Vietnamnet #Thờisự #PL</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vietnamnet.vn</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CÔ GIÁO 'DỖI' KHÔNG SOẠN ĐỀ CƯƠNG ÔN TẬP VÌ PHỤ HUYNH KHÔNG ĐỒNG Ý HỖ TRỢ LAPTOP
+Theo phản ánh, trong ngày họp phụ huynh đầu năm của lớp 4/3 (diễn ra ngày 14/9), cô H. đề nghị phụ huynh hỗ trợ 1 laptop trị giá 4-5 triệu đồng, máy in tài liệu và hỗ trợ cô bảo mẫu của lớp 300.000 đồng/tháng. Lúc đó, phụ huynh của lớp 4/3 có ý kiến rằng máy in đã được trang bị từ lớp 3, cô giáo nên liên hệ giáo viên chủ nhiệm cũ để xin lại cho lớp. 
+Phụ huynh trong lớp cũng tính toán rằng với chiếc laptop tầm 5-6 triệu đồng, mỗi người sẽ phải đóng góp từ 200.000-300.000 đồng. 
+Đến ngày 16/9, cô H. lại tiếp tục nhắn với nội dung: “Hôm thứ Bảy (14/9), cô có xin phụ huynh hỗ trợ cái máy laptop khoảng 5-6 triệu. Và cô đã mua cái máy 11 triệu thì cô bù vào 5 triệu. Cái laptop này là của cô, phụ huynh có đồng ý không?”.
+Sau đó, cô giáo này đã tạo bình chọn đồng ý và không đồng ý. Trong lúc bình chọn, khi thấy có phụ huynh không đồng ý, cô H. nhắn hỏi là phụ huynh của bé nào. 
+Cô giáo cho biết đã có phụ huynh không đồng ý thì cô sẽ không nhận cô cũng không phải soạn đề cương ôn tập cho các con.
+Nhiều phụ huynh nêu ý kiến rằng từ đầu năm đến nay, họ thấy con mình rất ít khi chép bài vì không theo kịp các nội dung trên Youtube. Đồng thời, cô giáo cũng không đồng ý kết bạn Zalo với phụ huynh để trao đổi về vấn đề học tập, không giảng dạy đúng theo thời khoá biểu, bán đồ ăn cho học sinh…
+Phụ huynh nêu rằng họ đã mất lòng tin ở cô H. nên không đồng ý giáo viên này tiếp tục giảng dạy ở lớp 4/3.
+Còn cô H. thì nói rằng bản thân đã làm phụ huynh hiểu lầm ý qua các tin nhắn trong nhóm Zalo của lớp. Cô cũng nhận sai khi vận động phụ huynh trang bị cho mình máy laptop và giữ tiền quỹ của lớp.
+“Tôi xin lỗi thầy hiệu trưởng, phụ huynh lớp 4/3. Tôi hứa sẽ sửa chữa sai lầm đã gây ra” - cô giáo nói.
+#Vietnamnet #Giáodục #PL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vietnamnet.vn</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>PHẠT KÊNH YOUTUBE “NHỮNG BÀI HỌC NHỎ” 15 TRIỆU ĐỒNG VÌ ĐĂNG VIDEO “QUẢ BÁO LÀNG NỦ” GIỮA LÚC LÀNG NỦ ĐANG CHÌM TRONG ĐAU THƯƠNG 
+Ngày 28/9, Công an TP Hà Nội cho biết, trước tình hình lũ lụt và bão số 3 gây thiệt hại tại nhiều địa phương vừa qua, một số người chưa nhận thức đầy đủ ảnh hưởng việc đăng tải, chia sẻ những thông tin không đúng sự thật trên mạng xã hội khiến dư luận bức xúc.
+Mới đây, Phòng An ninh mạng và phòng, chống tội phạm sử dụng công nghệ cao (Công an TP Hà Nội) đã phát hiện, xử lý vi phạm liên quan đến Công ty cổ phần truyền thông SUNRISE về hành vi quản lý, sử dụng kênh Youtube “Những Bài Học Nhỏ” đăng tải lên không gian mạng video có thông tin bịa đặt về Làng Nủ vào ngày 16/9, gây bức xúc trong dư luận nhân dân.
+Tại cơ quan công an, bà Đ.P.T, đại diện Công ty cổ phần truyền thông SUNRISE thừa nhận kênh “Những Bài Học Nhỏ” thuộc công ty quản lý đã đăng tải lên không gian mạng video là thông tin bịa đặt.
+Phòng An ninh mạng và phòng, chống tội phạm sử dụng công nghệ cao (Công an TP Hà Nội) đã ra quyết định xử phạt công ty cổ phần truyền thông SUNRISE về hành vi “cung cấp, chia sẻ thông tin bịa đặt, gây hoang mang dư luận trong nhân dân...” với mức phạt tiền là 15 triệu đồng.
+#Vietnamnet #Thờisự #PL</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vietnamnet.vn</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ĐỀ NGHỊ TẠM DỪNG THI CÔNG DỰ ÁN ĐƯỜNG VEN SÔNG: NGHIÊN CỨU PHƯƠNG ÁN NẮN ĐƯỜNG, GIỮ LẠI BIỆT THỰ CỔ 100 TUỔI Ở ĐỒNG NAI 
+Sở Xây dựng tỉnh Đồng Nai cho biết, đã có văn bản gửi các cơ quan chức năng liên quan đề nghị tạm dừng thi công dự án đường ven sông, đoạn đi qua khu vực biệt thự 100 tuổi của ông Võ Hà Thanh.
+Theo đó, qua kiểm tra thực tế, cơ quan chức năng ghi nhận đơn vị thi công đang triển khai các hoạt động xây dựng tại khu vực này. Do đó, Sở Xây dựng đề nghị Ban Quản lý dự án và UBND TP Biên Hòa chỉ đạo các đơn vị có liên quan tạm ngưng thi công đối với đoạn tuyến đi qua khu vực biệt thự cổ, đồng thời giữ nguyên hiện trạng và rào chắn khu vực này.
+ #Vietnamnet #Thờisự #NH</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vietnamnet.vn</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Thủ tướng: Miễn, giảm thuế và lãi vay cho người dân, doanh nghiệp bị bão lũ
+#Chínhtrị #NH</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Quân đội bay flycam phát hiện 2 vết nứt dài trăm mét ở Hà Giang</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NÓNG
+Iran dội tên lửa vào Israel</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Tạm cắt cầu phao Phong Châu do nước sông Hồng dâng cao nhằm đảm bảo an toàn cho người dân và phương tiện</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Mưa lớn kéo dài tại Lào Cai khiến thôn Làng Nủ lại bị chia cắt do sạt lở đất và lũ quét...</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Krathon duy trì cấp siêu bão trên Biển Đông, biển động dữ dội</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Ngày 1/10, phiên tòa xét xử bà Trương Mỹ Lan và 33 bị cáo khác tại Tập đoàn Vạn Thịnh Phát tiếp tục với phần xét hỏi.
+Liên quan việc bị cáo Trương Mỹ Lan xin lại 2 chiếc túi Hermes bạch tạng làm kỷ niệm, bị cáo Lan nói: "Hai chiếc túi có tiền cũng không mua được, nhưng tôi có được chúng là nhờ tên tuổi của Trương Mỹ Lan và Chu Lập Cơ, nếu không đủ uy tín trên thế giới thì không mua nổi."
+Bị cáo Trương Mỹ Lan cho rằng, 2 chiếc túi Hermes bạch tạng đi đấu giá thì rất lâu, không bằng bị cáo nói với con cháu đi kiếm tiền về chuộc lại.
+#vtcnews #socialnews #hoithocuocsong</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Krathon duy trì cấp siêu bão trên Biển Đông, biển động dữ dội</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Hà Nội: Uống nước ngọt miễn phí ở cổng trường, 12 học sinh nhập viện</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Tối 30/9, Ban giám hiệu Trường tiểu học Chương Dương thành lập nhanh tổ công tác gồm đại diện Phòng GD&amp;ĐT Quận 1, Cấp ủy, Ban giám hiệu, Công đoàn trường, Ban Thanh tra nhân dân đến tiếp xúc, động viên cô Hạnh.
+Ban giám hiệu trường đã đề nghị cô giáo Trương Phương Hạnh tường trình làm rõ những nội dung có liên quan đến cô đang được đang tải trên MXH và nộp trước 9h ngày 3/10.
+#vtcnews #socialnews #hoithocuocsong</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Tạm đình chỉ công tác Giám đốc Ban Quản lý dự án đầu tư xây dựng TP Hạ Long</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Trung tâm Dự báo khí tượng thuỷ văn quốc gia cho biết, sáng sớm nay 1/10, bão Krathon đi vào vùng biển phía Đông Bắc của khu vực Bắc Biển Đông, trở thành cơn bão số 5 trong năm 2024.
+Theo dự báo hiện tại, bão không có khả năng ảnh hưởng đến vùng ven biển và đất liền nước ta.
+#vtcnews #socialnews #hoithocuocsong</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Thủ tướng: Dùng flycam quét các điểm nguy cơ sạt lở để có biện pháp phòng ngừa</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Bộ GD&amp;ĐT đồng ý cho học sinh nghỉ Tết Nguyên đán 9 ngày</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Vụ cô giáo xin tiền mua laptop cá nhân ở TP.HCM: Sáng nay, 2/3 học sinh không đến lớp</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Trước tình hình mưa lũ phức tạp gây sạt lở đất đá, lực lượng chức năng xã Việt Vinh (huyện Bắc Quang, tỉnh Hà Giang) đã vận động di dời khẩn cấp 46 hộ dân với hơn 170 khẩu đến nơi an toàn.
+Theo đó, những hộ dân nằm trong khu vực nguy hiểm đã được di dời đến khu vực thôn Thượng Mỹ (cách điểm sạt lở tại Km51 Quốc lộ 2 khoảng 500 mét).
+#vtcnews #socialnews #hoithocuocsong</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Cảnh báo dông tố, sét, mưa đá và mưa lớn cục bộ nội thành Hà Nội khoảng từ 20 phút đến 3 giờ tới</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Hà Giang: Cháy chợ lớn trong đêm, dân bất lực nhìn biển lửa thiêu rụi nhiều tài sản</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://www.facebook.com/vtcnewsvn</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new data day 07/10/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/ketqua2.xlsx
+++ b/Data/Draft/ketqua2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12180"/>
+    <workbookView windowWidth="13545" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,148 +490,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -993,13 +986,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="67" customWidth="1"/>
-  </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
new update day 08/10/2024
</commit_message>
<xml_diff>
--- a/Data/Draft/ketqua2.xlsx
+++ b/Data/Draft/ketqua2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13545" windowHeight="12180"/>
+    <workbookView windowWidth="27945" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -986,10 +986,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="88.4285714285714" customWidth="1"/>
+    <col min="5" max="5" width="64.2857142857143" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>